<commit_message>
Modified a excel file
</commit_message>
<xml_diff>
--- a/Sameh.xlsx
+++ b/Sameh.xlsx
@@ -1,25 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Git-course-notes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E58CE6-5847-4CD2-B2A0-ADEBA4AEAB40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +68,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +345,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C4:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>2312</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>2153</v>
+      </c>
+    </row>
+    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4634</v>
+      </c>
+    </row>
+    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f>6+6+65</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>